<commit_message>
Przypisanie wartości oceny klubów do meczów w które te kluby biorą udział, dzięki temu możemy porównywać oceny do pary klubów, które będą odbywały ze sobą mecz, dodatkowo kosmetyczne zmiany w listach, usunięcie białych znaków, które tworzyły niepożądane efekty
</commit_message>
<xml_diff>
--- a/EkstraklasaMoc.xlsx
+++ b/EkstraklasaMoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projekt_na_studia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E2CD03-DC29-421A-A106-A49BADF89DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD7F3F2-DD4D-4EB9-8B98-5C209D7D7617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="2295" windowWidth="28710" windowHeight="15450" xr2:uid="{5C82AE5A-E1D8-4783-ADB3-CF59E3A57158}"/>
+    <workbookView xWindow="3390" yWindow="1305" windowWidth="28710" windowHeight="15450" xr2:uid="{5C82AE5A-E1D8-4783-ADB3-CF59E3A57158}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,11 +628,12 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>